<commit_message>
Adjusted the user input menu and changed a couple of "hard" filters.
</commit_message>
<xml_diff>
--- a/outputs/filtered_tvseries.xlsx
+++ b/outputs/filtered_tvseries.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,33 +498,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dragon Ball</t>
+          <t>Star Trek</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dragon Ball: Doragon bôru</t>
+          <t>Star Trek</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Adventure,Sci-Fi</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>8.5</v>
+        <v>8.4</v>
       </c>
       <c r="F2" t="n">
-        <v>69457</v>
+        <v>95298</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -533,11 +533,11 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1986</v>
+        <v>1966</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1989</t>
+          <t>1969</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -547,40 +547,40 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>tt0088509</t>
+          <t>tt0060028</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Simpsons</t>
+          <t>3rd Rock from the Sun</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The Simpsons</t>
+          <t>3rd Rock from the Sun</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Animation,Comedy</t>
+          <t>Comedy,Family,Sci-Fi</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>8.699999999999999</v>
+        <v>7.8</v>
       </c>
       <c r="F3" t="n">
-        <v>445923</v>
+        <v>56714</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -589,11 +589,11 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1989</v>
+        <v>1996</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>\N</t>
+          <t>2001</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -603,40 +603,40 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>tt0096697</t>
+          <t>tt0115082</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Batman: The Animated Series</t>
+          <t>Firefly</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Batman: The Animated Series</t>
+          <t>Firefly</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Adventure,Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>9</v>
+        <v>8.9</v>
       </c>
       <c r="F4" t="n">
-        <v>122969</v>
+        <v>286919</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -645,11 +645,11 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1992</v>
+        <v>2002</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1995</t>
+          <t>2003</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -659,36 +659,36 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>tt0103359</t>
+          <t>tt0303461</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>X-Men</t>
+          <t>Doctor Who</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>X-Men</t>
+          <t>Doctor Who</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Adventure,Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>8.4</v>
+        <v>8.5</v>
       </c>
       <c r="F5" t="n">
-        <v>51406</v>
+        <v>253049</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -701,11 +701,11 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1992</v>
+        <v>2005</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1997</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -715,36 +715,36 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>tt0103584</t>
+          <t>tt0436992</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Neon Genesis Evangelion</t>
+          <t>Westworld</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Shinseiki Evangelion</t>
+          <t>Westworld</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Action,Animation,Drama</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E6" t="n">
         <v>8.5</v>
       </c>
       <c r="F6" t="n">
-        <v>91876</v>
+        <v>542433</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -757,11 +757,11 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1995</v>
+        <v>2016</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -771,40 +771,40 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>tt0112159</t>
+          <t>tt0475784</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dexter's Laboratory</t>
+          <t>Foundation</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dexter's Laboratory</t>
+          <t>Foundation</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Adventure,Animation,Comedy</t>
+          <t>Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>7.9</v>
+        <v>7.6</v>
       </c>
       <c r="F7" t="n">
-        <v>55110</v>
+        <v>102802</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -813,11 +813,11 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1996</v>
+        <v>2021</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>\N</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -827,40 +827,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>tt0115157</t>
+          <t>tt0804484</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>King of the Hill</t>
+          <t>Alice in Borderland</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>King of the Hill</t>
+          <t>Imawa no Kuni no Arisu</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Animation,Comedy,Drama</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>7.5</v>
+        <v>7.7</v>
       </c>
       <c r="F8" t="n">
-        <v>60091</v>
+        <v>103584</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -869,11 +869,11 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1997</v>
+        <v>2020</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>\N</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -883,40 +883,40 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>tt0118375</t>
+          <t>tt10795658</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dragon Ball Z</t>
+          <t>Fringe</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dragon Ball Z: Doragon bôru zetto</t>
+          <t>Fringe</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>46</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>8.800000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="F9" t="n">
-        <v>92039</v>
+        <v>261614</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -925,11 +925,11 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1989</v>
+        <v>2008</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -939,40 +939,40 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>tt0121220</t>
+          <t>tt1119644</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>South Park</t>
+          <t>Severance</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>South Park</t>
+          <t>Severance</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Animation,Comedy</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E10" t="n">
         <v>8.699999999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>415102</v>
+        <v>230746</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>HK</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -981,7 +981,7 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1997</v>
+        <v>2022</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -995,40 +995,40 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>tt0121955</t>
+          <t>tt11280740</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Futurama</t>
+          <t>Dollhouse</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Futurama</t>
+          <t>Dollhouse</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>44</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Adventure,Animation,Comedy</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>8.5</v>
+        <v>7.7</v>
       </c>
       <c r="F11" t="n">
-        <v>267242</v>
+        <v>52420</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1037,11 +1037,11 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1999</v>
+        <v>2009</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>\N</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1051,40 +1051,40 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>tt0149460</t>
+          <t>tt1135300</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Family Guy</t>
+          <t>Star Trek: Strange New Worlds</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Family Guy</t>
+          <t>Star Trek: Strange New Worlds</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Animation,Comedy</t>
+          <t>Action,Adventure,Sci-Fi</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>8.1</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>371376</v>
+        <v>62182</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1999</v>
+        <v>2022</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1107,36 +1107,36 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>tt0182576</t>
+          <t>tt12327578</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SpongeBob SquarePants</t>
+          <t>Stargate Universe</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SpongeBob SquarePants</t>
+          <t>Stargate Universe</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>43</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Animation,Comedy,Family</t>
+          <t>Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>8.199999999999999</v>
+        <v>7.6</v>
       </c>
       <c r="F13" t="n">
-        <v>115810</v>
+        <v>53973</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1149,11 +1149,11 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1999</v>
+        <v>2009</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>\N</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1163,40 +1163,40 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>tt0206512</t>
+          <t>tt1286039</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cowboy Bebop</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kaubôi bibappu: Cowboy Bebop</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>42</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Sci-Fi,Thriller</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>8.9</v>
+        <v>6.8</v>
       </c>
       <c r="F14" t="n">
-        <v>147135</v>
+        <v>59598</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1205,11 +1205,11 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1998</v>
+        <v>2009</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1219,40 +1219,40 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>tt0213338</t>
+          <t>tt1307824</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Dragon Ball Z</t>
+          <t>Flashforward</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Dragon Ball Z</t>
+          <t>Flashforward</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>42</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>8.800000000000001</v>
+        <v>7.6</v>
       </c>
       <c r="F15" t="n">
-        <v>155559</v>
+        <v>62480</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1261,11 +1261,11 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1996</v>
+        <v>2009</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1275,36 +1275,36 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>tt0214341</t>
+          <t>tt1441135</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Courage the Cowardly Dog</t>
+          <t>Silo</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Courage the Cowardly Dog</t>
+          <t>Silo</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>49</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Adventure,Animation,Comedy</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>8.300000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="F16" t="n">
-        <v>52937</v>
+        <v>146984</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1317,11 +1317,11 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1999</v>
+        <v>2023</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>\N</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1331,40 +1331,40 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>tt0220880</t>
+          <t>tt14688458</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Justice League</t>
+          <t>Under the Dome</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Justice League</t>
+          <t>Under the Dome</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>43</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="F17" t="n">
-        <v>53407</v>
+        <v>114375</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1373,11 +1373,11 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>2001</v>
+        <v>2013</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1387,40 +1387,40 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>tt0275137</t>
+          <t>tt1553656</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Samurai Jack</t>
+          <t>The Man in the High Castle</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Samurai Jack</t>
+          <t>The Man in the High Castle</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Sci-Fi,Thriller</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>8.5</v>
+        <v>7.9</v>
       </c>
       <c r="F18" t="n">
-        <v>61738</v>
+        <v>114374</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1429,11 +1429,11 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>2001</v>
+        <v>2015</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1443,40 +1443,40 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>tt0278238</t>
+          <t>tt1740299</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Dragon Ball</t>
+          <t>Dark Matter</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Dragon Ball</t>
+          <t>Dark Matter</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>\N</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Sci-Fi,Thriller</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>8.5</v>
+        <v>7.7</v>
       </c>
       <c r="F19" t="n">
-        <v>67404</v>
+        <v>51733</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1485,11 +1485,11 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1995</v>
+        <v>2024</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>\N</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1499,40 +1499,40 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>tt0280249</t>
+          <t>tt19231492</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Berserk</t>
+          <t>Continuum</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kenpuu Denki Berserk</t>
+          <t>Continuum</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Sci-Fi,Thriller</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>8.699999999999999</v>
+        <v>7.6</v>
       </c>
       <c r="F20" t="n">
-        <v>60206</v>
+        <v>64623</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1541,11 +1541,11 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1997</v>
+        <v>2012</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1555,40 +1555,40 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>tt0318871</t>
+          <t>tt1954347</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>One Piece</t>
+          <t>Orphan Black</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>One Piece: Wan pîsu</t>
+          <t>Orphan Black</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>44</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Sci-Fi,Thriller</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F21" t="n">
-        <v>272091</v>
+        <v>119126</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1597,11 +1597,11 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1999</v>
+        <v>2013</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>\N</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1611,36 +1611,36 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>tt0388629</t>
+          <t>tt2234222</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>American Dad!</t>
+          <t>Utopia</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>American Dad!</t>
+          <t>Utopia</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Animation,Comedy</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7.4</v>
+        <v>8.4</v>
       </c>
       <c r="F22" t="n">
-        <v>138737</v>
+        <v>52552</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1653,11 +1653,11 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>2005</v>
+        <v>2013</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>\N</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1667,40 +1667,40 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>tt0397306</t>
+          <t>tt2384811</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Naruto</t>
+          <t>The Last Ship</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Naruto</t>
+          <t>The Last Ship</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>8.4</v>
+        <v>7.4</v>
       </c>
       <c r="F23" t="n">
-        <v>137749</v>
+        <v>65316</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1709,11 +1709,11 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>2002</v>
+        <v>2014</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1723,40 +1723,40 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>tt0409591</t>
+          <t>tt2402207</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Avatar: The Last Airbender</t>
+          <t>Sense8</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Avatar: The Last Airbender</t>
+          <t>Sense8</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>9.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="F24" t="n">
-        <v>391302</v>
+        <v>165774</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1765,11 +1765,11 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -1779,40 +1779,40 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>tt0417299</t>
+          <t>tt2431438</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Samurai Champloo</t>
+          <t>The 100</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Samurai Chanpurû</t>
+          <t>The 100</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>43</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="F25" t="n">
-        <v>57673</v>
+        <v>285240</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1821,11 +1821,11 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>2004</v>
+        <v>2014</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1835,40 +1835,40 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>tt0423731</t>
+          <t>tt2661044</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bleach</t>
+          <t>Halo</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bleach</t>
+          <t>Halo</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Adventure,Sci-Fi</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>8.199999999999999</v>
+        <v>7.3</v>
       </c>
       <c r="F26" t="n">
-        <v>76072</v>
+        <v>99554</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1877,11 +1877,11 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>2004</v>
+        <v>2022</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1891,40 +1891,40 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>tt0434665</t>
+          <t>tt2934286</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Monster</t>
+          <t>The Expanse</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Monster</t>
+          <t>The Expanse</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Animation,Crime,Drama</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>8.699999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="F27" t="n">
-        <v>51394</v>
+        <v>178189</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>HK</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1933,11 +1933,11 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>2004</v>
+        <v>2015</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -1947,36 +1947,36 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>tt0434706</t>
+          <t>tt3230854</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Star Wars: The Clone Wars</t>
+          <t>Fear the Walking Dead</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Star Wars: The Clone Wars</t>
+          <t>Fear the Walking Dead</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>44</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Horror,Sci-Fi</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>8.4</v>
+        <v>6.8</v>
       </c>
       <c r="F28" t="n">
-        <v>126898</v>
+        <v>147963</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1989,11 +1989,11 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2003,40 +2003,40 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>tt0458290</t>
+          <t>tt3743822</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Phineas and Ferb</t>
+          <t>Legion</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Phineas and Ferb</t>
+          <t>Legion</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>\N</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E29" t="n">
         <v>8.1</v>
       </c>
       <c r="F29" t="n">
-        <v>59856</v>
+        <v>99321</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2045,11 +2045,11 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>2007</v>
+        <v>2017</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2059,40 +2059,40 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>tt0852863</t>
+          <t>tt5114356</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Naruto: Shippuden</t>
+          <t>Travelers</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Naruto: Shippûden</t>
+          <t>Travelers</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>8.699999999999999</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
-        <v>184943</v>
+        <v>67143</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2101,11 +2101,11 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2115,40 +2115,40 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>tt0988824</t>
+          <t>tt5651844</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Code Geass</t>
+          <t>The Handmaid's Tale</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kôdo Giasu: Hangyaku no Rurûshu</t>
+          <t>The Handmaid's Tale</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Action,Animation,Drama</t>
+          <t>Drama,Sci-Fi,Thriller</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>8.699999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="F31" t="n">
-        <v>85838</v>
+        <v>265793</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2157,11 +2157,11 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>2006</v>
+        <v>2017</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2171,40 +2171,40 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>tt0994314</t>
+          <t>tt5834204</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>What If...?</t>
+          <t>Snowpiercer</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>What If...?</t>
+          <t>Snowpiercer</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>7.4</v>
+        <v>6.9</v>
       </c>
       <c r="F32" t="n">
-        <v>147775</v>
+        <v>67743</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2213,7 +2213,7 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2227,36 +2227,36 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>tt10168312</t>
+          <t>tt6156584</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Arcane</t>
+          <t>For All Mankind</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Arcane: League of Legends</t>
+          <t>For All Mankind</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>8.1</v>
       </c>
       <c r="F33" t="n">
-        <v>335383</v>
+        <v>75390</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2269,11 +2269,11 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>\N</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2283,40 +2283,40 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>tt11126994</t>
+          <t>tt7772588</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Jujutsu Kaisen</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Jujutsu Kaisen</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Comedy,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>8.5</v>
+        <v>7.8</v>
       </c>
       <c r="F34" t="n">
-        <v>136979</v>
+        <v>82419</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2339,40 +2339,40 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>tt12343534</t>
+          <t>tt7826376</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Star Wars: The Bad Batch</t>
+          <t>See</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Star Wars: The Bad Batch</t>
+          <t>See</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Action,Drama,Sci-Fi</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
       <c r="F35" t="n">
-        <v>58853</v>
+        <v>101967</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2381,11 +2381,11 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2395,40 +2395,40 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>tt12708542</t>
+          <t>tt7949218</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Blue Eye Samurai</t>
+          <t>The Peripheral</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Blue Eye Samurai</t>
+          <t>The Peripheral</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>60</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>8.699999999999999</v>
+        <v>7.6</v>
       </c>
       <c r="F36" t="n">
-        <v>82056</v>
+        <v>84686</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2437,11 +2437,11 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>\N</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2451,40 +2451,40 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>tt13309742</t>
+          <t>tt8291284</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Fullmetal Alchemist: Brotherhood</t>
+          <t>Manifest</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Hagane no renkinjutsushi</t>
+          <t>Manifest</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>43</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Action,Adventure,Animation</t>
+          <t>Drama,Mystery,Sci-Fi</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>9.1</v>
+        <v>7</v>
       </c>
       <c r="F37" t="n">
-        <v>209946</v>
+        <v>95290</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>HK</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2493,11 +2493,11 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>2009</v>
+        <v>2018</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -2507,40 +2507,40 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>tt1355642</t>
+          <t>tt8421350</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Chainsaw Man</t>
+          <t>Raised by Wolves</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Chainsaw Man</t>
+          <t>Raised by Wolves</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>55</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Animation,Thriller</t>
+          <t>Drama,Fantasy,Sci-Fi</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>8.300000000000001</v>
+        <v>7.4</v>
       </c>
       <c r="F38" t="n">
-        <v>66037</v>
+        <v>88942</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>HK</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2549,7 +2549,7 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -2563,1351 +2563,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>tt13616990</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Archer</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Archer</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Action,Animation,Comedy</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="F39" t="n">
-        <v>169344</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>HK</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I39" t="n">
-        <v>2009</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>tt1486217</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Bob's Burgers</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Bob's Burgers</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Animation,Comedy</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="F40" t="n">
-        <v>95619</v>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>EG</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I40" t="n">
-        <v>2011</v>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>tt1561755</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>The Legend of Korra</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>The Legend of Korra</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="F41" t="n">
-        <v>142181</v>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
-        <v>2012</v>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>tt1695360</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Regular Show</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Regular Show</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="F42" t="n">
-        <v>62654</v>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
-        <v>2010</v>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>tt1710308</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Gravity Falls</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Gravity Falls</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Adventure,Animation,Comedy</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>8.9</v>
-      </c>
-      <c r="F43" t="n">
-        <v>147802</v>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>HK</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I43" t="n">
-        <v>2012</v>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>tt1865718</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Steins;Gate</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Steins;Gate</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Animation,Comedy,Drama</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="F44" t="n">
-        <v>78426</v>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>HK</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I44" t="n">
-        <v>2011</v>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>tt1910272</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Hunter x Hunter</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Hunter x Hunter</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
-        <v>9</v>
-      </c>
-      <c r="F45" t="n">
-        <v>150386</v>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I45" t="n">
-        <v>2011</v>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>tt2098220</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Sword Art Online</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Sword Art Online</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="F46" t="n">
-        <v>55338</v>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>HK</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I46" t="n">
-        <v>2012</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>tt2250192</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Attack on Titan</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Shingeki no Kyojin</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>9.1</v>
-      </c>
-      <c r="F47" t="n">
-        <v>565962</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I47" t="n">
-        <v>2013</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>tt2560140</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Rick and Morty</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Rick and Morty</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Adventure,Animation,Comedy</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
-        <v>9.1</v>
-      </c>
-      <c r="F48" t="n">
-        <v>628969</v>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I48" t="n">
-        <v>2013</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>tt2861424</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Star Wars: Rebels</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Star Wars Rebels</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="F49" t="n">
-        <v>61270</v>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>2014</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>tt2930604</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Parasyte: The Maxim</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Kiseijû: Sei no kakuritsu</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Action,Animation,Drama</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="F50" t="n">
-        <v>52777</v>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>NZ</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I50" t="n">
-        <v>2014</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>tt3358020</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>BoJack Horseman</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>BoJack Horseman</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Animation,Comedy,Drama</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="F51" t="n">
-        <v>201009</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
-        <v>2014</v>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>tt3398228</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>One Punch Man</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>One Punch Man: Wanpanman</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Action,Animation,Comedy</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="F52" t="n">
-        <v>194475</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>PH</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I52" t="n">
-        <v>2015</v>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>tt4508902</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Disenchantment</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Disenchantment</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="F53" t="n">
-        <v>75134</v>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I53" t="n">
-        <v>2018</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>tt5363918</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>My Hero Academia</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Boku no hîrô akademia</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E54" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="F54" t="n">
-        <v>86518</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I54" t="n">
-        <v>2016</v>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>tt5626028</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Mob Psycho 100</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Mob Psycho 100</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Action,Animation,Comedy</t>
-        </is>
-      </c>
-      <c r="E55" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="F55" t="n">
-        <v>50673</v>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I55" t="n">
-        <v>2016</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>tt5897304</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Castlevania</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Castlevania</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="F56" t="n">
-        <v>84764</v>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>EG</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I56" t="n">
-        <v>2017</v>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>tt6517102</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Big Mouth</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Big Mouth</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Animation,Comedy,Romance</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="F57" t="n">
-        <v>91613</v>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>EG</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I57" t="n">
-        <v>2017</v>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>tt6524350</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Invincible</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Invincible</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E58" t="n">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="F58" t="n">
-        <v>222935</v>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>HK</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I58" t="n">
-        <v>2021</v>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>tt6741278</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>The Heroes</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>The Heroes</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Animation,Drama,History</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="F59" t="n">
-        <v>168745</v>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I59" t="n">
-        <v>2008</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>tt7657124</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>The Promised Neverland</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Yakusoku no Neverland</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Adventure,Animation,Drama</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="F60" t="n">
-        <v>50167</v>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I60" t="n">
-        <v>2019</v>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>tt8788458</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Demon Slayer: Kimetsu no Yaiba</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Kimetsu no Yaiba</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E61" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="F61" t="n">
-        <v>171997</v>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>2019</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>tt9335498</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Love, Death &amp; Robots</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Love, Death &amp; Robots</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Animation</t>
-        </is>
-      </c>
-      <c r="E62" t="n">
-        <v>8.4</v>
-      </c>
-      <c r="F62" t="n">
-        <v>206079</v>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>EG</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="I62" t="n">
-        <v>2019</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>\N</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>tvSeries</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>tt9561862</t>
+          <t>tt9170108</t>
         </is>
       </c>
     </row>

</xml_diff>